<commit_message>
remove enzyme treatment from sugarcane biorefineries; only relevant for old lipidcane biorefinery
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1_agile.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1_agile.xlsx
@@ -712,37 +712,37 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>-0.02520688468827538</v>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.007782661943306476</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.008223408328936331</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.3</v>
+        <v>0.003914455548578222</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.2</v>
+        <v>-0.007852005434080217</v>
       </c>
       <c r="I4" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.007427469321098772</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.8999999999999998</v>
+        <v>0.01547328433134627</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.2</v>
+        <v>-0.007325059589002383</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.2</v>
+        <v>-0.007325059589002383</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
-        <v>-0.2</v>
+        <v>-0.007325059589002383</v>
       </c>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
@@ -764,37 +764,37 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.6</v>
+        <v>0.0115595550543822</v>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>0.7999999999999999</v>
+        <v>-0.01407169025886761</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2</v>
+        <v>0.0007133395485335818</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.8999999999999998</v>
+        <v>0.01979438354377534</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.4999999999999999</v>
+        <v>0.005608826624353065</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.2</v>
+        <v>0.00101141024845641</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3</v>
+        <v>-0.01162842516101724</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.4999999999999999</v>
+        <v>0.005777384391095375</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.4999999999999999</v>
+        <v>0.005777384391095375</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>-0.4999999999999999</v>
+        <v>0.005777384391095375</v>
       </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
@@ -816,37 +816,37 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.2</v>
+        <v>0.1242969290678771</v>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.2397781137511245</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.8999999999999998</v>
+        <v>-0.9630775918351036</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3</v>
+        <v>-0.01103339948133598</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.9999985236159408</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8999999999999998</v>
+        <v>0.974571654918866</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.001146409098474829</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.998159780438391</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.998159780438391</v>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.998159780438391</v>
       </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
@@ -872,37 +872,37 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.9679153566046141</v>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>0.8999999999999998</v>
+        <v>-0.01554655732586229</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.0008166083846643351</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.7999999999999999</v>
+        <v>0.0129473774778951</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.2</v>
+        <v>0.005653261570130462</v>
       </c>
       <c r="I7" t="n">
-        <v>0.09999999999999999</v>
+        <v>0.002638555305542212</v>
       </c>
       <c r="J7" t="n">
-        <v>0.09999999999999999</v>
+        <v>0.02341774543165503</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.2</v>
+        <v>0.006539426661577065</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.2</v>
+        <v>0.006539426661577065</v>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
-        <v>-0.2</v>
+        <v>0.006539426661577065</v>
       </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
@@ -928,37 +928,37 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.8999999999999998</v>
+        <v>-0.01221661767266471</v>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.01610273526810941</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.2</v>
+        <v>0.008100074244002969</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.8999999999999998</v>
+        <v>-0.01662873100114924</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.01299195315967813</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2</v>
+        <v>-0.0102946025557841</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3</v>
+        <v>0.002334397337582074</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.01346264981850599</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.01346264981850599</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.01346264981850599</v>
       </c>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
@@ -984,37 +984,37 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.4999999999999999</v>
+        <v>0.01822791653711666</v>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>-0.3</v>
+        <v>0.008118562116742485</v>
       </c>
       <c r="F9" t="n">
-        <v>0.7</v>
+        <v>-0.02970020230800809</v>
       </c>
       <c r="G9" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.01572980117319205</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.6</v>
+        <v>0.02697309285492371</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.7</v>
+        <v>0.02904841143393645</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3</v>
+        <v>-0.006415171041820074</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.6</v>
+        <v>0.02638637059145482</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.6</v>
+        <v>0.02638637059145482</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>-0.6</v>
+        <v>0.02638637059145482</v>
       </c>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
@@ -1040,37 +1040,37 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.02995293355011733</v>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.00996457681458307</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8999999999999998</v>
+        <v>0.002169485654779426</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2</v>
+        <v>0.001081241707249668</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.7</v>
+        <v>-0.00188187050727482</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.8999999999999998</v>
+        <v>-0.001164699886587995</v>
       </c>
       <c r="J10" t="n">
-        <v>0.6</v>
+        <v>-0.01730201824222126</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.7</v>
+        <v>-0.002570364294814572</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.7</v>
+        <v>-0.002570364294814572</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>-0.7</v>
+        <v>-0.002570364294814572</v>
       </c>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
@@ -1092,37 +1092,37 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.7999999999999999</v>
+        <v>0.0682421952416878</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>0.8999999999999998</v>
+        <v>0.7349377253015089</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.2476595541303822</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.9999999999999999</v>
+        <v>-0.986848105553924</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.3</v>
+        <v>-0.005492080539683221</v>
       </c>
       <c r="I11" t="n">
-        <v>0.09999999999999999</v>
+        <v>0.2132218491688739</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>-0.003444746942869331</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.3</v>
+        <v>-0.03849618038784721</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.3</v>
+        <v>-0.03849618038784721</v>
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>-0.3</v>
+        <v>-0.03849618038784721</v>
       </c>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
@@ -1144,37 +1144,37 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.3</v>
+        <v>-0.195346674373867</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.0005569421982776878</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.00579465949578638</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.2</v>
+        <v>0.002669817706792708</v>
       </c>
       <c r="H12" t="n">
-        <v>0.3</v>
+        <v>0.007162120990484839</v>
       </c>
       <c r="I12" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.006233193849327753</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.6</v>
+        <v>0.02224051103150239</v>
       </c>
       <c r="K12" t="n">
-        <v>0.3</v>
+        <v>0.006510444164417765</v>
       </c>
       <c r="L12" t="n">
-        <v>0.3</v>
+        <v>0.006510444164417765</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>0.3</v>
+        <v>0.006510444164417765</v>
       </c>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
@@ -1200,37 +1200,37 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.01029115845964634</v>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>-0.02247291190691647</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7999999999999999</v>
+        <v>-0.007538661709546468</v>
       </c>
       <c r="G13" t="n">
-        <v>0.09999999999999999</v>
+        <v>0.02293552142942086</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.6</v>
+        <v>0.01388905399556216</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.7999999999999999</v>
+        <v>0.009781065223242607</v>
       </c>
       <c r="J13" t="n">
-        <v>0.7999999999999999</v>
+        <v>-0.001155375210786514</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.6</v>
+        <v>0.01559175316767012</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.6</v>
+        <v>0.01559175316767012</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>-0.6</v>
+        <v>0.01559175316767012</v>
       </c>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
@@ -1256,37 +1256,37 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.00437981326319253</v>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>-0.7</v>
+        <v>-0.01727859064314363</v>
       </c>
       <c r="F14" t="n">
-        <v>0.3</v>
+        <v>0.006693708363748334</v>
       </c>
       <c r="G14" t="n">
-        <v>0.8999999999999998</v>
+        <v>0.01574907528596301</v>
       </c>
       <c r="H14" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.003306701220268048</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.3</v>
+        <v>-0.006288456731538269</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2</v>
+        <v>-0.01784087026903606</v>
       </c>
       <c r="K14" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.002267557338702293</v>
       </c>
       <c r="L14" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.002267557338702293</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.002267557338702293</v>
       </c>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
@@ -1312,37 +1312,37 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.6</v>
+        <v>0.006973099862923994</v>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
-        <v>0.7999999999999999</v>
+        <v>0.005723682180947287</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2</v>
+        <v>0.01205131574605263</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.8999999999999998</v>
+        <v>0.0003351033734041349</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.01231107908444316</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.2</v>
+        <v>-0.01113809343752374</v>
       </c>
       <c r="J15" t="n">
-        <v>0.3</v>
+        <v>-0.03215043972383302</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.01252159672486387</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.01252159672486387</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.01252159672486387</v>
       </c>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -1368,37 +1368,37 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.6</v>
+        <v>0.02342736938509477</v>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
-        <v>-0.7999999999999999</v>
+        <v>0.01545196487407859</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.2</v>
+        <v>-0.01154427982177119</v>
       </c>
       <c r="G16" t="n">
-        <v>0.8999999999999998</v>
+        <v>-0.00507402452296098</v>
       </c>
       <c r="H16" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.009126217901048716</v>
       </c>
       <c r="I16" t="n">
-        <v>0.2</v>
+        <v>0.0114335949853438</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.3</v>
+        <v>-0.01444963310289037</v>
       </c>
       <c r="K16" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.008193815463752616</v>
       </c>
       <c r="L16" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.008193815463752616</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.008193815463752616</v>
       </c>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
@@ -1420,37 +1420,37 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.3</v>
+        <v>-0.0006896704595868182</v>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.01026630636265225</v>
       </c>
       <c r="F17" t="n">
-        <v>0.8999999999999998</v>
+        <v>0.009664435682577426</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3</v>
+        <v>0.002034194577367783</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.7999999999999999</v>
+        <v>-0.007901475196059007</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.8999999999999998</v>
+        <v>-0.006991911447676457</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.01456265703121181</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.7999999999999999</v>
+        <v>-0.006728304845132193</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.7999999999999999</v>
+        <v>-0.006728304845132193</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>-0.7999999999999999</v>
+        <v>-0.006728304845132193</v>
       </c>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
@@ -1476,37 +1476,37 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.7</v>
+        <v>-0.01939918445596737</v>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
-        <v>0.8999999999999998</v>
+        <v>0.01386254801050192</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.4999999999999999</v>
+        <v>0.004673633274945329</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.7</v>
+        <v>-0.005226530513061219</v>
       </c>
       <c r="H18" t="n">
-        <v>0.3</v>
+        <v>-0.00731511101260444</v>
       </c>
       <c r="I18" t="n">
-        <v>0.4999999999999999</v>
+        <v>-0.005049995625999825</v>
       </c>
       <c r="J18" t="n">
-        <v>0.4</v>
+        <v>-0.01042169579337634</v>
       </c>
       <c r="K18" t="n">
-        <v>0.3</v>
+        <v>-0.008199142215965688</v>
       </c>
       <c r="L18" t="n">
-        <v>0.3</v>
+        <v>-0.008199142215965688</v>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>0.3</v>
+        <v>-0.008199142215965688</v>
       </c>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
@@ -1532,37 +1532,37 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.01588151573926063</v>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
-        <v>-0.6</v>
+        <v>-0.002911123316444933</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.6</v>
+        <v>0.006796998799879952</v>
       </c>
       <c r="G19" t="n">
-        <v>0.7</v>
+        <v>-0.002696432267857291</v>
       </c>
       <c r="H19" t="n">
-        <v>0.7999999999999999</v>
+        <v>-0.0066431175137247</v>
       </c>
       <c r="I19" t="n">
-        <v>0.6</v>
+        <v>-0.005374445494977819</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.4</v>
+        <v>-0.01646803326647601</v>
       </c>
       <c r="K19" t="n">
-        <v>0.7999999999999999</v>
+        <v>-0.00675762478230499</v>
       </c>
       <c r="L19" t="n">
-        <v>0.7999999999999999</v>
+        <v>-0.00675762478230499</v>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>0.7999999999999999</v>
+        <v>-0.00675762478230499</v>
       </c>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
@@ -1584,37 +1584,37 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>0.008443730545749222</v>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
-        <v>0.2</v>
+        <v>0.01809021624360865</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.7999999999999999</v>
+        <v>0.006464746914589876</v>
       </c>
       <c r="G20" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.01337225410289016</v>
       </c>
       <c r="H20" t="n">
-        <v>0.8999999999999998</v>
+        <v>-0.009791524615660983</v>
       </c>
       <c r="I20" t="n">
-        <v>0.7999999999999999</v>
+        <v>-0.006784460047378401</v>
       </c>
       <c r="J20" t="n">
-        <v>0.3</v>
+        <v>0.006980377396312287</v>
       </c>
       <c r="K20" t="n">
-        <v>0.8999999999999998</v>
+        <v>-0.01081085179243407</v>
       </c>
       <c r="L20" t="n">
-        <v>0.8999999999999998</v>
+        <v>-0.01081085179243407</v>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>0.8999999999999998</v>
+        <v>-0.01081085179243407</v>
       </c>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
@@ -1636,37 +1636,37 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.7999999999999999</v>
+        <v>-0.007346701541868061</v>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.003649722289988891</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.009431244473249778</v>
       </c>
       <c r="G21" t="n">
-        <v>0.3</v>
+        <v>-0.004802896992115879</v>
       </c>
       <c r="H21" t="n">
-        <v>0.2</v>
+        <v>-0.009914377644575104</v>
       </c>
       <c r="I21" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.0100263775850551</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.01177479646290069</v>
       </c>
       <c r="K21" t="n">
-        <v>0.2</v>
+        <v>-0.00935579653423186</v>
       </c>
       <c r="L21" t="n">
-        <v>0.2</v>
+        <v>-0.00935579653423186</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>0.2</v>
+        <v>-0.00935579653423186</v>
       </c>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
@@ -1688,37 +1688,37 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.2</v>
+        <v>0.006930391861215674</v>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>0.001589515551580622</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.6</v>
+        <v>0.01709893393195736</v>
       </c>
       <c r="G22" t="n">
-        <v>0.3</v>
+        <v>-0.00361174900846996</v>
       </c>
       <c r="H22" t="n">
-        <v>0.7</v>
+        <v>-0.01984955349798214</v>
       </c>
       <c r="I22" t="n">
-        <v>0.6</v>
+        <v>-0.01796197329447893</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.005632457545436058</v>
       </c>
       <c r="K22" t="n">
-        <v>0.7</v>
+        <v>-0.01960951787238071</v>
       </c>
       <c r="L22" t="n">
-        <v>0.7</v>
+        <v>-0.01960951787238071</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>0.7</v>
+        <v>-0.01960951787238071</v>
       </c>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
@@ -1744,37 +1744,37 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.009002455944098238</v>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>-0.00257142375085695</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.2</v>
+        <v>0.01232098647683946</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.4</v>
+        <v>0.01631303652452146</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.008776817343072693</v>
       </c>
       <c r="I23" t="n">
-        <v>0.2</v>
+        <v>-0.01193964566158582</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.7</v>
+        <v>-0.02344283543262435</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.00894218301368732</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.00894218301368732</v>
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.00894218301368732</v>
       </c>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
@@ -1796,37 +1796,37 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.6</v>
+        <v>0.0007663044786521791</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
-        <v>0.7</v>
+        <v>0.01217688855107554</v>
       </c>
       <c r="F24" t="n">
-        <v>0.4999999999999999</v>
+        <v>-0.02449781301191252</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.6</v>
+        <v>-0.005227342673093706</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.6</v>
+        <v>0.02186211965848478</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.4999999999999999</v>
+        <v>0.02275960987038439</v>
       </c>
       <c r="J24" t="n">
-        <v>0.7</v>
+        <v>-0.005259561393981524</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.6</v>
+        <v>0.0209824675912987</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.6</v>
+        <v>0.0209824675912987</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>-0.6</v>
+        <v>0.0209824675912987</v>
       </c>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
@@ -1852,37 +1852,37 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.3</v>
+        <v>0.0240912826596513</v>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
-        <v>0.6</v>
+        <v>-0.007191037247641488</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.6</v>
+        <v>-0.009800704712028187</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.7</v>
+        <v>0.007577252943090117</v>
       </c>
       <c r="H25" t="n">
-        <v>0.3</v>
+        <v>0.01142455264898211</v>
       </c>
       <c r="I25" t="n">
-        <v>0.6</v>
+        <v>0.01117785644711426</v>
       </c>
       <c r="J25" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.01435854734231898</v>
       </c>
       <c r="K25" t="n">
-        <v>0.3</v>
+        <v>0.01178341544733662</v>
       </c>
       <c r="L25" t="n">
-        <v>0.3</v>
+        <v>0.01178341544733662</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
-        <v>0.3</v>
+        <v>0.01178341544733662</v>
       </c>
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
@@ -1904,37 +1904,37 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>-0.6</v>
+        <v>-0.01170576651623066</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>-0.7</v>
+        <v>-0.01469849578793983</v>
       </c>
       <c r="F26" t="n">
-        <v>-0.4999999999999999</v>
+        <v>0.01033753615750145</v>
       </c>
       <c r="G26" t="n">
-        <v>0.6</v>
+        <v>0.01766405216256208</v>
       </c>
       <c r="H26" t="n">
-        <v>0.6</v>
+        <v>-0.005179425807177031</v>
       </c>
       <c r="I26" t="n">
-        <v>0.4999999999999999</v>
+        <v>-0.009274533202981328</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.7</v>
+        <v>0.01880119663886984</v>
       </c>
       <c r="K26" t="n">
-        <v>0.6</v>
+        <v>-0.004281952683278106</v>
       </c>
       <c r="L26" t="n">
-        <v>0.6</v>
+        <v>-0.004281952683278106</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>0.6</v>
+        <v>-0.004281952683278106</v>
       </c>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
@@ -1960,37 +1960,37 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.4</v>
+        <v>0.01502293327291733</v>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>0.3</v>
+        <v>-0.03465603959424158</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.3</v>
+        <v>-0.01713647281345891</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.6</v>
+        <v>0.004103097956123918</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.02207754165110166</v>
       </c>
       <c r="I27" t="n">
-        <v>0.3</v>
+        <v>0.01994497692579908</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.7999999999999999</v>
+        <v>0.01058199059041446</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.02462607045704282</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.02462607045704282</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.02462607045704282</v>
       </c>
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
@@ -2016,37 +2016,37 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>-0.004767116638684665</v>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.01506191666647666</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.006258648250345929</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.3</v>
+        <v>-0.008269908234796328</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.2</v>
+        <v>-0.008266401258656049</v>
       </c>
       <c r="I28" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.008308641836345672</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.8999999999999998</v>
+        <v>-0.004181471191781383</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.2</v>
+        <v>-0.008948820357952813</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.2</v>
+        <v>-0.008948820357952813</v>
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="n">
-        <v>-0.2</v>
+        <v>-0.008948820357952813</v>
       </c>
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
@@ -2072,37 +2072,37 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.3</v>
+        <v>-0.005609890496395618</v>
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.02586618785064751</v>
       </c>
       <c r="F29" t="n">
-        <v>0.4999999999999999</v>
+        <v>-0.01980953378438135</v>
       </c>
       <c r="G29" t="n">
-        <v>0.3</v>
+        <v>-0.007308810436352417</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.2</v>
+        <v>0.01749584383583375</v>
       </c>
       <c r="I29" t="n">
-        <v>-0.4999999999999999</v>
+        <v>0.01698371127134845</v>
       </c>
       <c r="J29" t="n">
-        <v>0.8999999999999998</v>
+        <v>0.01847455664723586</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.2</v>
+        <v>0.01490515307620612</v>
       </c>
       <c r="L29" t="n">
-        <v>-0.2</v>
+        <v>0.01490515307620612</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="n">
-        <v>-0.2</v>
+        <v>0.01490515307620612</v>
       </c>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
@@ -2128,37 +2128,37 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.005613895904555835</v>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
-        <v>-0.3</v>
+        <v>0.01918661644746465</v>
       </c>
       <c r="F30" t="n">
-        <v>0.7</v>
+        <v>0.01417785570311422</v>
       </c>
       <c r="G30" t="n">
-        <v>0.4999999999999999</v>
+        <v>-0.01238681281547251</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.4</v>
+        <v>-0.01718398916735956</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.7</v>
+        <v>-0.01571460946058437</v>
       </c>
       <c r="J30" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.007748158357410279</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.4</v>
+        <v>-0.01813534190941367</v>
       </c>
       <c r="L30" t="n">
-        <v>-0.4</v>
+        <v>-0.01813534190941367</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="n">
-        <v>-0.4</v>
+        <v>-0.01813534190941367</v>
       </c>
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
@@ -2184,37 +2184,37 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.3</v>
+        <v>0.01884732968189318</v>
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>0.09999999999999999</v>
+        <v>0.01824520181780807</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.0190875325395013</v>
       </c>
       <c r="G31" t="n">
-        <v>0.3</v>
+        <v>-0.0005945371437814855</v>
       </c>
       <c r="H31" t="n">
-        <v>0.3</v>
+        <v>-0.02042824804912992</v>
       </c>
       <c r="I31" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.02022070112882804</v>
       </c>
       <c r="J31" t="n">
-        <v>0.4</v>
+        <v>-0.002456968714847717</v>
       </c>
       <c r="K31" t="n">
-        <v>0.3</v>
+        <v>-0.02154230697369227</v>
       </c>
       <c r="L31" t="n">
-        <v>0.3</v>
+        <v>-0.02154230697369227</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
-        <v>0.3</v>
+        <v>-0.02154230697369227</v>
       </c>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
@@ -2240,37 +2240,37 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>-0.6</v>
+        <v>0.006831829809273191</v>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
-        <v>-0.2</v>
+        <v>-0.007914755740590227</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>0.01092167150886686</v>
       </c>
       <c r="G32" t="n">
-        <v>0.09999999999999999</v>
+        <v>0.01206494093059764</v>
       </c>
       <c r="H32" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.007686408691456347</v>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>-0.01066486276259451</v>
       </c>
       <c r="J32" t="n">
-        <v>0.3</v>
+        <v>-0.01635629014271284</v>
       </c>
       <c r="K32" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.007525910509036419</v>
       </c>
       <c r="L32" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.007525910509036419</v>
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.007525910509036419</v>
       </c>
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
@@ -2296,37 +2296,37 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.8999999999999998</v>
+        <v>-0.02805956521838261</v>
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="n">
-        <v>0.7</v>
+        <v>-0.02234691276587651</v>
       </c>
       <c r="F33" t="n">
-        <v>0.3</v>
+        <v>0.0009205416368216654</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.6</v>
+        <v>0.02809268310770732</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.4999999999999999</v>
+        <v>0.004991588455663538</v>
       </c>
       <c r="I33" t="n">
-        <v>-0.3</v>
+        <v>-0.0002478960099158403</v>
       </c>
       <c r="J33" t="n">
-        <v>0.2</v>
+        <v>-0.02975334152411836</v>
       </c>
       <c r="K33" t="n">
-        <v>-0.4999999999999999</v>
+        <v>0.005963607310544291</v>
       </c>
       <c r="L33" t="n">
-        <v>-0.4999999999999999</v>
+        <v>0.005963607310544291</v>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
-        <v>-0.4999999999999999</v>
+        <v>0.005963607310544291</v>
       </c>
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
@@ -2352,37 +2352,37 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-0.6</v>
+        <v>-0.01327298856291954</v>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="n">
-        <v>-0.4999999999999999</v>
+        <v>-0.0004143562725742508</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.7</v>
+        <v>-0.01256295717451828</v>
       </c>
       <c r="G34" t="n">
-        <v>0.6</v>
+        <v>-0.007547552653902105</v>
       </c>
       <c r="H34" t="n">
-        <v>0.8999999999999998</v>
+        <v>0.009961462382458494</v>
       </c>
       <c r="I34" t="n">
-        <v>0.7</v>
+        <v>0.01112760610910424</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.2</v>
+        <v>-0.0008376853340178389</v>
       </c>
       <c r="K34" t="n">
-        <v>0.8999999999999998</v>
+        <v>0.01027877445915098</v>
       </c>
       <c r="L34" t="n">
-        <v>0.8999999999999998</v>
+        <v>0.01027877445915098</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
-        <v>0.8999999999999998</v>
+        <v>0.01027877445915098</v>
       </c>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
@@ -2408,37 +2408,37 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>-0.6</v>
+        <v>0.0162348474973939</v>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>-0.3</v>
+        <v>0.02612780658111226</v>
       </c>
       <c r="F35" t="n">
-        <v>0.3</v>
+        <v>-0.02187856321114252</v>
       </c>
       <c r="G35" t="n">
-        <v>0.4</v>
+        <v>-0.02810160870806434</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>0.01638748279949931</v>
       </c>
       <c r="I35" t="n">
-        <v>-0.3</v>
+        <v>0.02121788081671523</v>
       </c>
       <c r="J35" t="n">
-        <v>0.7</v>
+        <v>-0.00639943378213678</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>0.01455211805408472</v>
       </c>
       <c r="L35" t="n">
-        <v>0</v>
+        <v>0.01455211805408472</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="n">
-        <v>0</v>
+        <v>0.01455211805408472</v>
       </c>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
@@ -2464,37 +2464,37 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>0.02282898148915926</v>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
-        <v>-0.09999999999999999</v>
+        <v>-0.002307951356318054</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.002517871972714878</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.3</v>
+        <v>0.001494377915775116</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.2</v>
+        <v>-0.001649435297977412</v>
       </c>
       <c r="I36" t="n">
-        <v>0.09999999999999999</v>
+        <v>-0.002243779097751163</v>
       </c>
       <c r="J36" t="n">
-        <v>-0.8999999999999998</v>
+        <v>0.006495649534634759</v>
       </c>
       <c r="K36" t="n">
-        <v>-0.2</v>
+        <v>-0.001343303573732143</v>
       </c>
       <c r="L36" t="n">
-        <v>-0.2</v>
+        <v>-0.001343303573732143</v>
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
-        <v>-0.2</v>
+        <v>-0.001343303573732143</v>
       </c>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
@@ -2520,37 +2520,37 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.6</v>
+        <v>0.01849582105983284</v>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
-        <v>0.3</v>
+        <v>-0.008949108453964337</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.3</v>
+        <v>0.01616912887076515</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.4</v>
+        <v>0.01710014084400563</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>-0.01259444555977782</v>
       </c>
       <c r="I37" t="n">
-        <v>0.3</v>
+        <v>-0.01429813353192534</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.7</v>
+        <v>0.002181480533989604</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>-0.01190055714802228</v>
       </c>
       <c r="L37" t="n">
-        <v>0</v>
+        <v>-0.01190055714802228</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
-        <v>0</v>
+        <v>-0.01190055714802228</v>
       </c>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>

</xml_diff>

<commit_message>
rerun some simulations, prepare more figs for manuscript
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1_agile.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-1_agile.xlsx
@@ -734,7 +734,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.00048208600328344</v>
+        <v>0.0005490377499615099</v>
       </c>
       <c r="D4" t="n">
         <v>0.001852952042118082</v>
@@ -743,35 +743,37 @@
       <c r="F4" t="n">
         <v>0.01414777467791099</v>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>0.1723324617869151</v>
+      </c>
       <c r="H4" t="n">
         <v>-0.01416035989441439</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0002168657366746295</v>
+        <v>-0.0001601380864055235</v>
       </c>
       <c r="J4" t="n">
-        <v>0.01592108798976341</v>
+        <v>0.01396881377040935</v>
       </c>
       <c r="K4" t="n">
-        <v>0.00724631203385248</v>
+        <v>-0.02000815875232635</v>
       </c>
       <c r="L4" t="n">
-        <v>0.00724631203385248</v>
+        <v>-0.02000815875232635</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
-        <v>0.00724631203385248</v>
+        <v>-0.02000815875232635</v>
       </c>
       <c r="P4" t="n">
-        <v>0.00724631203385248</v>
+        <v>-0.0200080201283208</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.00724631203385248</v>
+        <v>-0.02000812956832518</v>
       </c>
       <c r="R4" t="n">
-        <v>0.00724631203385248</v>
+        <v>-0.02000812956832518</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
@@ -795,7 +797,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.006564532390581295</v>
+        <v>-0.006568123942724957</v>
       </c>
       <c r="D5" t="n">
         <v>-0.01802875377715015</v>
@@ -804,35 +806,37 @@
       <c r="F5" t="n">
         <v>-0.01678080134323205</v>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>-0.005485724199142705</v>
+      </c>
       <c r="H5" t="n">
         <v>0.01674125778965031</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.01553196042927842</v>
+        <v>-0.0155212701568508</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.01442324309578888</v>
+        <v>-0.01169165793331156</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.01555594535823781</v>
+        <v>-0.01279277791971111</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.01555594535823781</v>
+        <v>-0.01279277791971111</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="n">
-        <v>-0.01555594535823781</v>
+        <v>-0.01279277791971111</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.01555594535823781</v>
+        <v>-0.01279810822392433</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.01555594535823781</v>
+        <v>-0.01279469475178779</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.01555594535823781</v>
+        <v>-0.01279469475178779</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
@@ -856,7 +860,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1731066082682643</v>
+        <v>0.1731025307641012</v>
       </c>
       <c r="D6" t="n">
         <v>0.9745858367114333</v>
@@ -865,35 +869,37 @@
       <c r="F6" t="n">
         <v>-0.01190033654001346</v>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>0.01245345074180139</v>
+      </c>
       <c r="H6" t="n">
         <v>0.01410731720429269</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9999999958719997</v>
+        <v>0.999997630815905</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0002543893355872565</v>
+        <v>0.004338874818659215</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.01342926053717042</v>
+        <v>-0.01318204651128186</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.01342926053717042</v>
+        <v>-0.01318204651128186</v>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
-        <v>-0.01342926053717042</v>
+        <v>-0.01318204651128186</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.01342926053717042</v>
+        <v>-0.01321424433656977</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.01342926053717042</v>
+        <v>-0.01318574635142985</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.01342926053717042</v>
+        <v>-0.01318574635142985</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
@@ -921,7 +927,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9639628104625123</v>
+        <v>0.9639626386225055</v>
       </c>
       <c r="D7" t="n">
         <v>0.02393805868552234</v>
@@ -930,35 +936,37 @@
       <c r="F7" t="n">
         <v>0.006647556649902265</v>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>0.004169662978761648</v>
+      </c>
       <c r="H7" t="n">
         <v>-0.00661536477661459</v>
       </c>
       <c r="I7" t="n">
-        <v>0.02276984836679393</v>
+        <v>0.02276107454244298</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.009001567571485621</v>
+        <v>-0.007485336698754165</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.001005679720227189</v>
+        <v>0.0007116180764647229</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.001005679720227189</v>
+        <v>0.0007116180764647229</v>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="n">
-        <v>-0.001005679720227189</v>
+        <v>0.0007116180764647229</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.001005679720227189</v>
+        <v>0.0007200428448017138</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.001005679720227189</v>
+        <v>0.000712020124480805</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.001005679720227189</v>
+        <v>0.000712020124480805</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
@@ -986,7 +994,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.02889608189184327</v>
+        <v>-0.028906025188241</v>
       </c>
       <c r="D8" t="n">
         <v>-0.01610414560416582</v>
@@ -995,35 +1003,37 @@
       <c r="F8" t="n">
         <v>-0.0233435725177429</v>
       </c>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>-0.0209525683889148</v>
+      </c>
       <c r="H8" t="n">
         <v>0.02333347994133919</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.01257291083891643</v>
+        <v>-0.01253378046935122</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.00272921009581338</v>
+        <v>-0.002512979418980495</v>
       </c>
       <c r="K8" t="n">
-        <v>0.007927918493116737</v>
+        <v>0.01132633197305328</v>
       </c>
       <c r="L8" t="n">
-        <v>0.007927918493116737</v>
+        <v>0.01132633197305328</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="n">
-        <v>0.007927918493116737</v>
+        <v>0.01132633197305328</v>
       </c>
       <c r="P8" t="n">
-        <v>0.007927918493116737</v>
+        <v>0.01132871142914846</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.007927918493116737</v>
+        <v>0.01132491405299656</v>
       </c>
       <c r="R8" t="n">
-        <v>0.007927918493116737</v>
+        <v>0.01132491405299656</v>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
@@ -1051,7 +1061,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.004383885295355411</v>
+        <v>-0.004389476047579041</v>
       </c>
       <c r="D9" t="n">
         <v>0.01773055731722229</v>
@@ -1060,35 +1070,37 @@
       <c r="F9" t="n">
         <v>-0.01403518424140737</v>
       </c>
-      <c r="G9" t="inlineStr"/>
+      <c r="G9" t="n">
+        <v>0.007478138160984351</v>
+      </c>
       <c r="H9" t="n">
         <v>0.01407902360316094</v>
       </c>
       <c r="I9" t="n">
-        <v>0.02048295192331807</v>
+        <v>0.02045288078611523</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0112910132865705</v>
+        <v>0.01134154438863928</v>
       </c>
       <c r="K9" t="n">
-        <v>0.007566856814674272</v>
+        <v>0.006049082353963293</v>
       </c>
       <c r="L9" t="n">
-        <v>0.007566856814674272</v>
+        <v>0.006049082353963293</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="n">
-        <v>0.007566856814674272</v>
+        <v>0.006049082353963293</v>
       </c>
       <c r="P9" t="n">
-        <v>0.007566856814674272</v>
+        <v>0.006043576369743054</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.007566856814674272</v>
+        <v>0.0060497475379899</v>
       </c>
       <c r="R9" t="n">
-        <v>0.007566856814674272</v>
+        <v>0.0060497475379899</v>
       </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
@@ -1116,7 +1128,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.03478861348754454</v>
+        <v>0.0347961725278469</v>
       </c>
       <c r="D10" t="n">
         <v>-0.001247748721909949</v>
@@ -1125,35 +1137,37 @@
       <c r="F10" t="n">
         <v>-0.01138696067947842</v>
       </c>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="n">
+        <v>0.01841776207785618</v>
+      </c>
       <c r="H10" t="n">
         <v>0.01141014813640592</v>
       </c>
       <c r="I10" t="n">
-        <v>0.001682647363305894</v>
+        <v>0.00164121376164855</v>
       </c>
       <c r="J10" t="n">
-        <v>0.006093003907308991</v>
+        <v>0.00434404839232288</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.0157222825488913</v>
+        <v>-0.01939215024768601</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.0157222825488913</v>
+        <v>-0.01939215024768601</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="n">
-        <v>-0.0157222825488913</v>
+        <v>-0.01939215024768601</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.0157222825488913</v>
+        <v>-0.01939966483998659</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.0157222825488913</v>
+        <v>-0.0193933426637337</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.0157222825488913</v>
+        <v>-0.0193933426637337</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
@@ -1177,7 +1191,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.08052294638891784</v>
+        <v>0.08052745627709824</v>
       </c>
       <c r="D11" t="n">
         <v>0.204425199857008</v>
@@ -1186,35 +1200,37 @@
       <c r="F11" t="n">
         <v>0.9999969645758784</v>
       </c>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="n">
+        <v>0.01522939623123428</v>
+      </c>
       <c r="H11" t="n">
         <v>-0.9999999996159999</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.01410315838812633</v>
+        <v>-0.0141244675089787</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.01310088580880346</v>
+        <v>-0.01308733346872416</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.341696325347853</v>
+        <v>-0.338395951391838</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.341696325347853</v>
+        <v>-0.338395951391838</v>
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="n">
-        <v>-0.341696325347853</v>
+        <v>-0.338395951391838</v>
       </c>
       <c r="P11" t="n">
-        <v>-0.341696325347853</v>
+        <v>-0.3383511112300444</v>
       </c>
       <c r="Q11" t="n">
-        <v>-0.341696325347853</v>
+        <v>-0.3383913830396553</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.341696325347853</v>
+        <v>-0.3383913830396553</v>
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
@@ -1238,7 +1254,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.1821351636374065</v>
+        <v>-0.1821366331094653</v>
       </c>
       <c r="D12" t="n">
         <v>-5.44318101772724e-05</v>
@@ -1247,35 +1263,37 @@
       <c r="F12" t="n">
         <v>0.0113231701169268</v>
       </c>
-      <c r="G12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>-0.01791790050225182</v>
+      </c>
       <c r="H12" t="n">
         <v>-0.0113262949170518</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.002222479960899198</v>
+        <v>-0.002170712726828509</v>
       </c>
       <c r="J12" t="n">
-        <v>0.004285416574319378</v>
+        <v>0.00385600381301615</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0251769375830775</v>
+        <v>0.02850299989211999</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0251769375830775</v>
+        <v>0.02850299989211999</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="n">
-        <v>0.0251769375830775</v>
+        <v>0.02850299989211999</v>
       </c>
       <c r="P12" t="n">
-        <v>0.0251769375830775</v>
+        <v>0.02851550331662013</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.0251769375830775</v>
+        <v>0.02850422542816901</v>
       </c>
       <c r="R12" t="n">
-        <v>0.0251769375830775</v>
+        <v>0.02850422542816901</v>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
@@ -1303,7 +1321,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.00608704853148194</v>
+        <v>-0.006075666195026648</v>
       </c>
       <c r="D13" t="n">
         <v>-0.01226342717853708</v>
@@ -1312,35 +1330,37 @@
       <c r="F13" t="n">
         <v>-0.0008882437795297511</v>
       </c>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>0.03446967087839847</v>
+      </c>
       <c r="H13" t="n">
         <v>0.000879233603169344</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.01320984552039382</v>
+        <v>-0.01328595230743809</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.0008374703963824075</v>
+        <v>-0.002566190609396088</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.006328967197158687</v>
+        <v>-0.01066434196257368</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.006328967197158687</v>
+        <v>-0.01066434196257368</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="n">
-        <v>-0.006328967197158687</v>
+        <v>-0.01066434196257368</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.006328967197158687</v>
+        <v>-0.01066500081060003</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.006328967197158687</v>
+        <v>-0.01066508145060326</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.006328967197158687</v>
+        <v>-0.01066508145060326</v>
       </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
@@ -1368,7 +1388,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.01012472853298914</v>
+        <v>0.01012963643718546</v>
       </c>
       <c r="D14" t="n">
         <v>-0.001213954320558173</v>
@@ -1377,35 +1397,37 @@
       <c r="F14" t="n">
         <v>0.005412363096494523</v>
       </c>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>0.0111200608694498</v>
+      </c>
       <c r="H14" t="n">
         <v>-0.005427399097095963</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.002982794135311765</v>
+        <v>-0.002997566423902657</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.01674803079147271</v>
+        <v>-0.01673818014287778</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.0009124272364970893</v>
+        <v>-0.004195027655801106</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.0009124272364970893</v>
+        <v>-0.004195027655801106</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="n">
-        <v>-0.0009124272364970893</v>
+        <v>-0.004195027655801106</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.0009124272364970893</v>
+        <v>-0.004186783079471322</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.0009124272364970893</v>
+        <v>-0.004192730375709214</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.0009124272364970893</v>
+        <v>-0.004192730375709214</v>
       </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
@@ -1433,7 +1455,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.01366610425864417</v>
+        <v>-0.0136689099547564</v>
       </c>
       <c r="D15" t="n">
         <v>-0.009827577321103093</v>
@@ -1442,35 +1464,37 @@
       <c r="F15" t="n">
         <v>-0.002109005364360214</v>
       </c>
-      <c r="G15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>-0.02159705013619393</v>
+      </c>
       <c r="H15" t="n">
         <v>0.002040708369628334</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.009771036582841461</v>
+        <v>-0.009729030245161209</v>
       </c>
       <c r="J15" t="n">
-        <v>0.01555366432162807</v>
+        <v>0.01799112011354024</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.01860157735206309</v>
+        <v>-0.01406483528259341</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.01860157735206309</v>
+        <v>-0.01406483528259341</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>-0.01860157735206309</v>
+        <v>-0.01406483528259341</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.01860157735206309</v>
+        <v>-0.014063950066558</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.01860157735206309</v>
+        <v>-0.0140644900665796</v>
       </c>
       <c r="R15" t="n">
-        <v>-0.01860157735206309</v>
+        <v>-0.0140644900665796</v>
       </c>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
@@ -1498,7 +1522,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.01075405550216222</v>
+        <v>0.01075729828629193</v>
       </c>
       <c r="D16" t="n">
         <v>0.0003126309245052369</v>
@@ -1507,35 +1531,37 @@
       <c r="F16" t="n">
         <v>0.01179920130396805</v>
       </c>
-      <c r="G16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>0.01307729363204273</v>
+      </c>
       <c r="H16" t="n">
         <v>-0.01178561951142478</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.002993346359733854</v>
+        <v>-0.003017124696684987</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.02061981893952328</v>
+        <v>-0.01453876988011651</v>
       </c>
       <c r="K16" t="n">
-        <v>0.03741997445679898</v>
+        <v>0.03433117135724685</v>
       </c>
       <c r="L16" t="n">
-        <v>0.03741997445679898</v>
+        <v>0.03433117135724685</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="n">
-        <v>0.03741997445679898</v>
+        <v>0.03433117135724685</v>
       </c>
       <c r="P16" t="n">
-        <v>0.03741997445679898</v>
+        <v>0.03432783612511343</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.03741997445679898</v>
+        <v>0.03433089938923597</v>
       </c>
       <c r="R16" t="n">
-        <v>0.03741997445679898</v>
+        <v>0.03433089938923597</v>
       </c>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
@@ -1559,7 +1585,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.01398200187128007</v>
+        <v>0.01398000391920015</v>
       </c>
       <c r="D17" t="n">
         <v>0.02873018217320728</v>
@@ -1568,35 +1594,37 @@
       <c r="F17" t="n">
         <v>0.005981925071277001</v>
       </c>
-      <c r="G17" t="inlineStr"/>
+      <c r="G17" t="n">
+        <v>-0.003918442784618797</v>
+      </c>
       <c r="H17" t="n">
         <v>-0.005911380332455212</v>
       </c>
       <c r="I17" t="n">
-        <v>0.02929354139574165</v>
+        <v>0.02930505170020206</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.01327516317465129</v>
+        <v>-0.01116499537690213</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.005378558423142336</v>
+        <v>-0.003000830424033216</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.005378558423142336</v>
+        <v>-0.003000830424033216</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
-        <v>-0.005378558423142336</v>
+        <v>-0.003000830424033216</v>
       </c>
       <c r="P17" t="n">
-        <v>-0.005378558423142336</v>
+        <v>-0.003001184280047371</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.005378558423142336</v>
+        <v>-0.003002111640084465</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.005378558423142336</v>
+        <v>-0.003002111640084465</v>
       </c>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
@@ -1624,7 +1652,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.0165318325332733</v>
+        <v>0.01652900053316002</v>
       </c>
       <c r="D18" t="n">
         <v>0.004774460542978422</v>
@@ -1633,35 +1661,37 @@
       <c r="F18" t="n">
         <v>0.002715848364633934</v>
       </c>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>0.006024345950446289</v>
+      </c>
       <c r="H18" t="n">
         <v>-0.002708579916343196</v>
       </c>
       <c r="I18" t="n">
-        <v>0.004249531369981254</v>
+        <v>0.004233849865353994</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.02122400168013746</v>
+        <v>-0.01990193702504037</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.01655805848632234</v>
+        <v>-0.01787957130718285</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.01655805848632234</v>
+        <v>-0.01787957130718285</v>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>-0.01655805848632234</v>
+        <v>-0.01787957130718285</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.01655805848632234</v>
+        <v>-0.01788252157930086</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.01655805848632234</v>
+        <v>-0.01787891601115664</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.01655805848632234</v>
+        <v>-0.01787891601115664</v>
       </c>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
@@ -1689,7 +1719,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.002954748022189921</v>
+        <v>-0.002945047605801904</v>
       </c>
       <c r="D19" t="n">
         <v>0.003085432347417293</v>
@@ -1698,35 +1728,37 @@
       <c r="F19" t="n">
         <v>0.009961971566478862</v>
       </c>
-      <c r="G19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>0.01517551773485723</v>
+      </c>
       <c r="H19" t="n">
         <v>-0.009979181775167269</v>
       </c>
       <c r="I19" t="n">
-        <v>0.002071322194852888</v>
+        <v>0.002038242225529689</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.009927727477871287</v>
+        <v>-0.009420295417137072</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.003839863641594545</v>
+        <v>-0.006874429810977191</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.003839863641594545</v>
+        <v>-0.006874429810977191</v>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="n">
-        <v>-0.003839863641594545</v>
+        <v>-0.006874429810977191</v>
       </c>
       <c r="P19" t="n">
-        <v>-0.003839863641594545</v>
+        <v>-0.006882129011285159</v>
       </c>
       <c r="Q19" t="n">
-        <v>-0.003839863641594545</v>
+        <v>-0.006873350674934026</v>
       </c>
       <c r="R19" t="n">
-        <v>-0.003839863641594545</v>
+        <v>-0.006873350674934026</v>
       </c>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
@@ -1750,7 +1782,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.01417384539895382</v>
+        <v>-0.0141754050150162</v>
       </c>
       <c r="D20" t="n">
         <v>0.0005019740360789613</v>
@@ -1759,35 +1791,37 @@
       <c r="F20" t="n">
         <v>0.002182366167294647</v>
       </c>
-      <c r="G20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>-0.00186224951279211</v>
+      </c>
       <c r="H20" t="n">
         <v>-0.00217547951101918</v>
       </c>
       <c r="I20" t="n">
-        <v>0.001037567849502714</v>
+        <v>0.001036024553440982</v>
       </c>
       <c r="J20" t="n">
-        <v>0.004450799227297439</v>
+        <v>0.003085129570384976</v>
       </c>
       <c r="K20" t="n">
-        <v>0.01639165073566603</v>
+        <v>0.01545686961027478</v>
       </c>
       <c r="L20" t="n">
-        <v>0.01639165073566603</v>
+        <v>0.01545686961027478</v>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>0.01639165073566603</v>
+        <v>0.01545686961027478</v>
       </c>
       <c r="P20" t="n">
-        <v>0.01639165073566603</v>
+        <v>0.01545258282610331</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.01639165073566603</v>
+        <v>0.01545623802624952</v>
       </c>
       <c r="R20" t="n">
-        <v>0.01639165073566603</v>
+        <v>0.01545623802624952</v>
       </c>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
@@ -1811,7 +1845,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.02366908030676321</v>
+        <v>0.02366182539447301</v>
       </c>
       <c r="D21" t="n">
         <v>-0.002844156401766256</v>
@@ -1820,35 +1854,37 @@
       <c r="F21" t="n">
         <v>-0.00781790853671634</v>
       </c>
-      <c r="G21" t="inlineStr"/>
+      <c r="G21" t="n">
+        <v>-0.01331993737312407</v>
+      </c>
       <c r="H21" t="n">
         <v>0.007782412343296493</v>
       </c>
       <c r="I21" t="n">
-        <v>6.886445075457803e-05</v>
+        <v>9.552249982089998e-05</v>
       </c>
       <c r="J21" t="n">
-        <v>0.002818569010992524</v>
+        <v>-0.002017125467082913</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.01686429734657189</v>
+        <v>-0.01386388788255551</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.01686429734657189</v>
+        <v>-0.01386388788255551</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>-0.01686429734657189</v>
+        <v>-0.01386388788255551</v>
       </c>
       <c r="P21" t="n">
-        <v>-0.01686429734657189</v>
+        <v>-0.01385716365828655</v>
       </c>
       <c r="Q21" t="n">
-        <v>-0.01686429734657189</v>
+        <v>-0.01386353661854146</v>
       </c>
       <c r="R21" t="n">
-        <v>-0.01686429734657189</v>
+        <v>-0.01386353661854146</v>
       </c>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
@@ -1872,7 +1908,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.03409716693188668</v>
+        <v>0.03409355896374235</v>
       </c>
       <c r="D22" t="n">
         <v>0.01360946550437862</v>
@@ -1881,35 +1917,37 @@
       <c r="F22" t="n">
         <v>-0.01723582446543298</v>
       </c>
-      <c r="G22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>-0.01283217023124631</v>
+      </c>
       <c r="H22" t="n">
         <v>0.0172887850755514</v>
       </c>
       <c r="I22" t="n">
-        <v>0.01792453156498126</v>
+        <v>0.01795447579017903</v>
       </c>
       <c r="J22" t="n">
-        <v>0.002274080613815726</v>
+        <v>0.001374194117552867</v>
       </c>
       <c r="K22" t="n">
-        <v>0.005955724846228992</v>
+        <v>0.006492440131697604</v>
       </c>
       <c r="L22" t="n">
-        <v>0.005955724846228992</v>
+        <v>0.006492440131697604</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="n">
-        <v>0.005955724846228992</v>
+        <v>0.006492440131697604</v>
       </c>
       <c r="P22" t="n">
-        <v>0.005955724846228992</v>
+        <v>0.006500370404014815</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.005955724846228992</v>
+        <v>0.00649455625978225</v>
       </c>
       <c r="R22" t="n">
-        <v>0.005955724846228992</v>
+        <v>0.00649455625978225</v>
       </c>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
@@ -1937,7 +1975,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>-0.0004409499056379962</v>
+        <v>-0.0004493382899735315</v>
       </c>
       <c r="D23" t="n">
         <v>-0.003054536282181451</v>
@@ -1946,35 +1984,37 @@
       <c r="F23" t="n">
         <v>-0.01822552997702119</v>
       </c>
-      <c r="G23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>-0.02062742631619378</v>
+      </c>
       <c r="H23" t="n">
         <v>0.01821622104864884</v>
       </c>
       <c r="I23" t="n">
-        <v>-0.000429987377199495</v>
+        <v>-0.0003873350554934022</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.002213067391375968</v>
+        <v>-0.005943813750777254</v>
       </c>
       <c r="K23" t="n">
-        <v>0.001706706116268245</v>
+        <v>0.003118949404757976</v>
       </c>
       <c r="L23" t="n">
-        <v>0.001706706116268245</v>
+        <v>0.003118949404757976</v>
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="n">
-        <v>0.001706706116268245</v>
+        <v>0.003118949404757976</v>
       </c>
       <c r="P23" t="n">
-        <v>0.001706706116268245</v>
+        <v>0.003107228476289138</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.001706706116268245</v>
+        <v>0.003116945788677831</v>
       </c>
       <c r="R23" t="n">
-        <v>0.001706706116268245</v>
+        <v>0.003116945788677831</v>
       </c>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
@@ -1998,7 +2038,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.003523877612955104</v>
+        <v>0.003523488812939552</v>
       </c>
       <c r="D24" t="n">
         <v>-0.002413117152524686</v>
@@ -2007,35 +2047,37 @@
       <c r="F24" t="n">
         <v>0.01382188788087551</v>
       </c>
-      <c r="G24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>-0.01792190199288719</v>
+      </c>
       <c r="H24" t="n">
         <v>-0.01384410420176417</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.006487587811503511</v>
+        <v>-0.006447042977881717</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.0008248143737297015</v>
+        <v>-0.0002639762639318813</v>
       </c>
       <c r="K24" t="n">
-        <v>0.006409586656383465</v>
+        <v>0.007966253214650125</v>
       </c>
       <c r="L24" t="n">
-        <v>0.006409586656383465</v>
+        <v>0.007966253214650125</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="n">
-        <v>0.006409586656383465</v>
+        <v>0.007966253214650125</v>
       </c>
       <c r="P24" t="n">
-        <v>0.006409586656383465</v>
+        <v>0.007962534558501381</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.006409586656383465</v>
+        <v>0.007965815838632633</v>
       </c>
       <c r="R24" t="n">
-        <v>0.006409586656383465</v>
+        <v>0.007965815838632633</v>
       </c>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
@@ -2063,7 +2105,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.02202483361699334</v>
+        <v>0.02202281176091247</v>
       </c>
       <c r="D25" t="n">
         <v>0.01544696836187873</v>
@@ -2072,35 +2114,37 @@
       <c r="F25" t="n">
         <v>-0.0001003973800158952</v>
       </c>
-      <c r="G25" t="inlineStr"/>
+      <c r="G25" t="n">
+        <v>-0.007685922671437729</v>
+      </c>
       <c r="H25" t="n">
         <v>0.0001228353649134146</v>
       </c>
       <c r="I25" t="n">
-        <v>0.015508450028338</v>
+        <v>0.01552019457280778</v>
       </c>
       <c r="J25" t="n">
-        <v>-0.01148018167573577</v>
+        <v>-0.009517524271934835</v>
       </c>
       <c r="K25" t="n">
-        <v>0.01686780864271235</v>
+        <v>0.01588065989922639</v>
       </c>
       <c r="L25" t="n">
-        <v>0.01686780864271235</v>
+        <v>0.01588065989922639</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="n">
-        <v>0.01686780864271235</v>
+        <v>0.01588065989922639</v>
       </c>
       <c r="P25" t="n">
-        <v>0.01686780864271235</v>
+        <v>0.01588398044335921</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.01686780864271235</v>
+        <v>0.01588130962725239</v>
       </c>
       <c r="R25" t="n">
-        <v>0.01686780864271235</v>
+        <v>0.01588130962725239</v>
       </c>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
@@ -2124,7 +2168,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.003214684736587389</v>
+        <v>0.003215428160617126</v>
       </c>
       <c r="D26" t="n">
         <v>-0.01184227429769097</v>
@@ -2133,35 +2177,37 @@
       <c r="F26" t="n">
         <v>0.0364560526262421</v>
       </c>
-      <c r="G26" t="inlineStr"/>
+      <c r="G26" t="n">
+        <v>-0.002682748942661645</v>
+      </c>
       <c r="H26" t="n">
         <v>-0.03650762958830518</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.0198560050822402</v>
+        <v>-0.01984707343388293</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.01543440381974499</v>
+        <v>-0.01605154503690799</v>
       </c>
       <c r="K26" t="n">
-        <v>0.001088339275533571</v>
+        <v>0.00176858301474332</v>
       </c>
       <c r="L26" t="n">
-        <v>0.001088339275533571</v>
+        <v>0.00176858301474332</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="n">
-        <v>0.001088339275533571</v>
+        <v>0.00176858301474332</v>
       </c>
       <c r="P26" t="n">
-        <v>0.001088339275533571</v>
+        <v>0.001772937478917499</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.001088339275533571</v>
+        <v>0.001767468166698726</v>
       </c>
       <c r="R26" t="n">
-        <v>0.001088339275533571</v>
+        <v>0.001767468166698726</v>
       </c>
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
@@ -2189,7 +2235,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>-0.001546515037860601</v>
+        <v>-0.001545012637800505</v>
       </c>
       <c r="D27" t="n">
         <v>0.007680210739208429</v>
@@ -2198,35 +2244,37 @@
       <c r="F27" t="n">
         <v>-0.001224724080988963</v>
       </c>
-      <c r="G27" t="inlineStr"/>
+      <c r="G27" t="n">
+        <v>0.003463491932336744</v>
+      </c>
       <c r="H27" t="n">
         <v>0.001241321617652864</v>
       </c>
       <c r="I27" t="n">
-        <v>0.008573812758952509</v>
+        <v>0.008571080982843237</v>
       </c>
       <c r="J27" t="n">
-        <v>0.006165225752215947</v>
+        <v>0.002774212446398408</v>
       </c>
       <c r="K27" t="n">
-        <v>0.02521534440061377</v>
+        <v>0.02712797110111884</v>
       </c>
       <c r="L27" t="n">
-        <v>0.02521534440061377</v>
+        <v>0.02712797110111884</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="n">
-        <v>0.02521534440061377</v>
+        <v>0.02712797110111884</v>
       </c>
       <c r="P27" t="n">
-        <v>0.02521534440061377</v>
+        <v>0.02714764822190592</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.02521534440061377</v>
+        <v>0.02712908038116321</v>
       </c>
       <c r="R27" t="n">
-        <v>0.02521534440061377</v>
+        <v>0.02712908038116321</v>
       </c>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
@@ -2254,7 +2302,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.007679476243179049</v>
+        <v>0.007674377490975098</v>
       </c>
       <c r="D28" t="n">
         <v>0.02252746592509864</v>
@@ -2263,35 +2311,37 @@
       <c r="F28" t="n">
         <v>-0.01371180736447229</v>
       </c>
-      <c r="G28" t="inlineStr"/>
+      <c r="G28" t="n">
+        <v>-0.01039149434307089</v>
+      </c>
       <c r="H28" t="n">
         <v>0.01375725328629013</v>
       </c>
       <c r="I28" t="n">
-        <v>0.02712407676496307</v>
+        <v>0.02714291666971666</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.02374199062139487</v>
+        <v>-0.02356659123012774</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.001891751691670067</v>
+        <v>0.001667368194694728</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.001891751691670067</v>
+        <v>0.001667368194694728</v>
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="n">
-        <v>-0.001891751691670067</v>
+        <v>0.001667368194694728</v>
       </c>
       <c r="P28" t="n">
-        <v>-0.001891751691670067</v>
+        <v>0.001655944194237767</v>
       </c>
       <c r="Q28" t="n">
-        <v>-0.001891751691670067</v>
+        <v>0.0016656950106278</v>
       </c>
       <c r="R28" t="n">
-        <v>-0.001891751691670067</v>
+        <v>0.0016656950106278</v>
       </c>
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
@@ -2319,7 +2369,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.00588653101946124</v>
+        <v>-0.00589253274770131</v>
       </c>
       <c r="D29" t="n">
         <v>0.01502535189701407</v>
@@ -2328,35 +2378,37 @@
       <c r="F29" t="n">
         <v>-0.009579881375195253</v>
       </c>
-      <c r="G29" t="inlineStr"/>
+      <c r="G29" t="n">
+        <v>0.002797867207601502</v>
+      </c>
       <c r="H29" t="n">
         <v>0.009623474880938994</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01756662934266517</v>
+        <v>0.01756315711852628</v>
       </c>
       <c r="J29" t="n">
-        <v>0.01499205225380917</v>
+        <v>0.01279555301050782</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.01868272989930919</v>
+        <v>-0.0196568376182735</v>
       </c>
       <c r="L29" t="n">
-        <v>-0.01868272989930919</v>
+        <v>-0.0196568376182735</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="n">
-        <v>-0.01868272989930919</v>
+        <v>-0.0196568376182735</v>
       </c>
       <c r="P29" t="n">
-        <v>-0.01868272989930919</v>
+        <v>-0.01965423486616939</v>
       </c>
       <c r="Q29" t="n">
-        <v>-0.01868272989930919</v>
+        <v>-0.01965646600225864</v>
       </c>
       <c r="R29" t="n">
-        <v>-0.01868272989930919</v>
+        <v>-0.01965646600225864</v>
       </c>
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
@@ -2384,7 +2436,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.01598172476726899</v>
+        <v>0.01598336934333477</v>
       </c>
       <c r="D30" t="n">
         <v>-0.03485036933001476</v>
@@ -2393,35 +2445,37 @@
       <c r="F30" t="n">
         <v>0.002960880118435204</v>
       </c>
-      <c r="G30" t="inlineStr"/>
+      <c r="G30" t="n">
+        <v>5.391275428393133e-05</v>
+      </c>
       <c r="H30" t="n">
         <v>-0.003049456249978249</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.03700981021639241</v>
+        <v>-0.03701771648870866</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.0006831943077571266</v>
+        <v>-0.002081952356001357</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.02886528125061125</v>
+        <v>-0.02816915459876618</v>
       </c>
       <c r="L30" t="n">
-        <v>-0.02886528125061125</v>
+        <v>-0.02816915459876618</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="n">
-        <v>-0.02886528125061125</v>
+        <v>-0.02816915459876618</v>
       </c>
       <c r="P30" t="n">
-        <v>-0.02886528125061125</v>
+        <v>-0.02817218368688734</v>
       </c>
       <c r="Q30" t="n">
-        <v>-0.02886528125061125</v>
+        <v>-0.02816784487071379</v>
       </c>
       <c r="R30" t="n">
-        <v>-0.02886528125061125</v>
+        <v>-0.02816784487071379</v>
       </c>
       <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr"/>
@@ -2449,7 +2503,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>-0.006957910646316424</v>
+        <v>-0.006952827350113093</v>
       </c>
       <c r="D31" t="n">
         <v>-0.02383454149738166</v>
@@ -2458,35 +2512,37 @@
       <c r="F31" t="n">
         <v>0.00230284674811387</v>
       </c>
-      <c r="G31" t="inlineStr"/>
+      <c r="G31" t="n">
+        <v>0.01056412996254546</v>
+      </c>
       <c r="H31" t="n">
         <v>-0.00237980601519224</v>
       </c>
       <c r="I31" t="n">
-        <v>-0.02427412090696483</v>
+        <v>-0.02430113876404555</v>
       </c>
       <c r="J31" t="n">
-        <v>0.01418349465709087</v>
+        <v>0.01802576952773132</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.001341177077647083</v>
+        <v>-0.000698452827938113</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.001341177077647083</v>
+        <v>-0.000698452827938113</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
-        <v>-0.001341177077647083</v>
+        <v>-0.000698452827938113</v>
       </c>
       <c r="P31" t="n">
-        <v>-0.001341177077647083</v>
+        <v>-0.0006978160599126422</v>
       </c>
       <c r="Q31" t="n">
-        <v>-0.001341177077647083</v>
+        <v>-0.0006983681559347261</v>
       </c>
       <c r="R31" t="n">
-        <v>-0.001341177077647083</v>
+        <v>-0.0006983681559347261</v>
       </c>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
@@ -2514,7 +2570,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.01636908987076359</v>
+        <v>0.01636200123048005</v>
       </c>
       <c r="D32" t="n">
         <v>-0.003733192661327706</v>
@@ -2523,35 +2579,37 @@
       <c r="F32" t="n">
         <v>0.01274513321380533</v>
       </c>
-      <c r="G32" t="inlineStr"/>
+      <c r="G32" t="n">
+        <v>-0.03026843770658894</v>
+      </c>
       <c r="H32" t="n">
         <v>-0.01276819798272792</v>
       </c>
       <c r="I32" t="n">
-        <v>-0.00698336802333472</v>
+        <v>-0.00692267653290706</v>
       </c>
       <c r="J32" t="n">
-        <v>0.0005190864927033493</v>
+        <v>0.0003208240509650233</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.003365314502612579</v>
+        <v>0.0025189775087591</v>
       </c>
       <c r="L32" t="n">
-        <v>-0.003365314502612579</v>
+        <v>0.0025189775087591</v>
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="n">
-        <v>-0.003365314502612579</v>
+        <v>0.0025189775087591</v>
       </c>
       <c r="P32" t="n">
-        <v>-0.003365314502612579</v>
+        <v>0.002518625092745004</v>
       </c>
       <c r="Q32" t="n">
-        <v>-0.003365314502612579</v>
+        <v>0.002518073668722946</v>
       </c>
       <c r="R32" t="n">
-        <v>-0.003365314502612579</v>
+        <v>0.002518073668722946</v>
       </c>
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr"/>
@@ -2579,7 +2637,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.01714243422169737</v>
+        <v>0.01715851172634046</v>
       </c>
       <c r="D33" t="n">
         <v>0.01683506400140256</v>
@@ -2588,35 +2646,37 @@
       <c r="F33" t="n">
         <v>-0.01379905677596227</v>
       </c>
-      <c r="G33" t="inlineStr"/>
+      <c r="G33" t="n">
+        <v>0.02662560730285095</v>
+      </c>
       <c r="H33" t="n">
         <v>0.01383685524147421</v>
       </c>
       <c r="I33" t="n">
-        <v>0.01915323916612956</v>
+        <v>0.01909827954793118</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.01722719210178852</v>
+        <v>-0.02100386744002722</v>
       </c>
       <c r="K33" t="n">
-        <v>0.005384327639373105</v>
+        <v>0.001639364321574573</v>
       </c>
       <c r="L33" t="n">
-        <v>0.005384327639373105</v>
+        <v>0.001639364321574573</v>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
-        <v>0.005384327639373105</v>
+        <v>0.001639364321574573</v>
       </c>
       <c r="P33" t="n">
-        <v>0.005384327639373105</v>
+        <v>0.001650623586024943</v>
       </c>
       <c r="Q33" t="n">
-        <v>0.005384327639373105</v>
+        <v>0.001638915233556609</v>
       </c>
       <c r="R33" t="n">
-        <v>0.005384327639373105</v>
+        <v>0.001638915233556609</v>
       </c>
       <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr"/>
@@ -2644,7 +2704,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.00935212703008508</v>
+        <v>0.009351921206076847</v>
       </c>
       <c r="D34" t="n">
         <v>-0.01617811696712467</v>
@@ -2653,35 +2713,37 @@
       <c r="F34" t="n">
         <v>-0.004008662464346498</v>
       </c>
-      <c r="G34" t="inlineStr"/>
+      <c r="G34" t="n">
+        <v>-0.001349632298006397</v>
+      </c>
       <c r="H34" t="n">
         <v>0.003972973022918921</v>
       </c>
       <c r="I34" t="n">
-        <v>-0.01603610339344413</v>
+        <v>-0.0160358949774358</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.01606456772267639</v>
+        <v>-0.01728817658704401</v>
       </c>
       <c r="K34" t="n">
-        <v>-0.009638295649531826</v>
+        <v>-0.009866475754659029</v>
       </c>
       <c r="L34" t="n">
-        <v>-0.009638295649531826</v>
+        <v>-0.009866475754659029</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="n">
-        <v>-0.009638295649531826</v>
+        <v>-0.009866475754659029</v>
       </c>
       <c r="P34" t="n">
-        <v>-0.009638295649531826</v>
+        <v>-0.009868109770724389</v>
       </c>
       <c r="Q34" t="n">
-        <v>-0.009638295649531826</v>
+        <v>-0.009866540362661614</v>
       </c>
       <c r="R34" t="n">
-        <v>-0.009638295649531826</v>
+        <v>-0.009866540362661614</v>
       </c>
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
@@ -2709,7 +2771,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.01299895856795834</v>
+        <v>0.01299776672791067</v>
       </c>
       <c r="D35" t="n">
         <v>0.01409742545989702</v>
@@ -2718,35 +2780,37 @@
       <c r="F35" t="n">
         <v>0.00260319725612789</v>
       </c>
-      <c r="G35" t="inlineStr"/>
+      <c r="G35" t="n">
+        <v>0.00125619566736742</v>
+      </c>
       <c r="H35" t="n">
         <v>-0.002598699559947982</v>
       </c>
       <c r="I35" t="n">
-        <v>0.01410030651601226</v>
+        <v>0.01409657566786303</v>
       </c>
       <c r="J35" t="n">
-        <v>0.004862266374880644</v>
+        <v>0.006656887628326019</v>
       </c>
       <c r="K35" t="n">
-        <v>0.01352840530913621</v>
+        <v>0.01288787187551487</v>
       </c>
       <c r="L35" t="n">
-        <v>0.01352840530913621</v>
+        <v>0.01288787187551487</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="n">
-        <v>0.01352840530913621</v>
+        <v>0.01288787187551487</v>
       </c>
       <c r="P35" t="n">
-        <v>0.01352840530913621</v>
+        <v>0.01288782589151303</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.01352840530913621</v>
+        <v>0.01288757677150307</v>
       </c>
       <c r="R35" t="n">
-        <v>0.01352840530913621</v>
+        <v>0.01288757677150307</v>
       </c>
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr"/>
@@ -2774,7 +2838,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.004608709432348377</v>
+        <v>0.004605885880235435</v>
       </c>
       <c r="D36" t="n">
         <v>-0.01006508315460332</v>
@@ -2783,35 +2847,37 @@
       <c r="F36" t="n">
         <v>0.01384931719397269</v>
       </c>
-      <c r="G36" t="inlineStr"/>
+      <c r="G36" t="n">
+        <v>0.004636316666257512</v>
+      </c>
       <c r="H36" t="n">
         <v>-0.01387379325895173</v>
       </c>
       <c r="I36" t="n">
-        <v>-0.01342120124084805</v>
+        <v>-0.01343607615344304</v>
       </c>
       <c r="J36" t="n">
-        <v>0.00676485223438375</v>
+        <v>0.009373038247763414</v>
       </c>
       <c r="K36" t="n">
-        <v>0.00682856628914265</v>
+        <v>0.01031599087663963</v>
       </c>
       <c r="L36" t="n">
-        <v>0.00682856628914265</v>
+        <v>0.01031599087663963</v>
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="n">
-        <v>0.00682856628914265</v>
+        <v>0.01031599087663963</v>
       </c>
       <c r="P36" t="n">
-        <v>0.00682856628914265</v>
+        <v>0.01032898322915933</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.00682856628914265</v>
+        <v>0.01031668870066755</v>
       </c>
       <c r="R36" t="n">
-        <v>0.00682856628914265</v>
+        <v>0.01031668870066755</v>
       </c>
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr"/>
@@ -2839,7 +2905,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>-0.01511947241277889</v>
+        <v>-0.01512009017280361</v>
       </c>
       <c r="D37" t="n">
         <v>0.01336814357472574</v>
@@ -2848,35 +2914,37 @@
       <c r="F37" t="n">
         <v>0.005984730383389214</v>
       </c>
-      <c r="G37" t="inlineStr"/>
+      <c r="G37" t="n">
+        <v>0.003564365592484008</v>
+      </c>
       <c r="H37" t="n">
         <v>-0.005943335181733406</v>
       </c>
       <c r="I37" t="n">
-        <v>0.01261250152850006</v>
+        <v>0.01261829551273182</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.01469904388758953</v>
+        <v>-0.01368536349532971</v>
       </c>
       <c r="K37" t="n">
-        <v>-0.005386508759460349</v>
+        <v>-0.006018210576728423</v>
       </c>
       <c r="L37" t="n">
-        <v>-0.005386508759460349</v>
+        <v>-0.006018210576728423</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="n">
-        <v>-0.005386508759460349</v>
+        <v>-0.006018210576728423</v>
       </c>
       <c r="P37" t="n">
-        <v>-0.005386508759460349</v>
+        <v>-0.006012491664499665</v>
       </c>
       <c r="Q37" t="n">
-        <v>-0.005386508759460349</v>
+        <v>-0.006017668944706758</v>
       </c>
       <c r="R37" t="n">
-        <v>-0.005386508759460349</v>
+        <v>-0.006017668944706758</v>
       </c>
       <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr"/>
@@ -2904,7 +2972,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>-0.009584389727375589</v>
+        <v>-0.009587140607485622</v>
       </c>
       <c r="D38" t="n">
         <v>-0.02239686339187453</v>
@@ -2913,35 +2981,37 @@
       <c r="F38" t="n">
         <v>-0.01842747049709882</v>
       </c>
-      <c r="G38" t="inlineStr"/>
+      <c r="G38" t="n">
+        <v>-0.01116464990267091</v>
+      </c>
       <c r="H38" t="n">
         <v>0.01837995347119814</v>
       </c>
       <c r="I38" t="n">
-        <v>-0.01924781520191261</v>
+        <v>-0.01922570716902828</v>
       </c>
       <c r="J38" t="n">
-        <v>0.01635715349626132</v>
+        <v>0.01846806149612711</v>
       </c>
       <c r="K38" t="n">
-        <v>0.9432969066278761</v>
+        <v>0.9255233631009344</v>
       </c>
       <c r="L38" t="n">
-        <v>0.9432969066278761</v>
+        <v>0.9255233631009344</v>
       </c>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="n">
-        <v>0.9432969066278761</v>
+        <v>0.9255233631009344</v>
       </c>
       <c r="P38" t="n">
-        <v>0.9432969066278761</v>
+        <v>0.9255003692760146</v>
       </c>
       <c r="Q38" t="n">
-        <v>0.9432969066278761</v>
+        <v>0.9255231248289248</v>
       </c>
       <c r="R38" t="n">
-        <v>0.9432969066278761</v>
+        <v>0.9255231248289248</v>
       </c>
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>

</xml_diff>